<commit_message>
inbevtradmx sand - fix some issues
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX_SAND/Data/inbevtradmx_template_2.xlsx
+++ b/Projects/INBEVTRADMX_SAND/Data/inbevtradmx_template_2.xlsx
@@ -20,13 +20,14 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">template!$A$1:$U$51</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$50</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$50</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="189">
   <si>
     <t xml:space="preserve">KPI Level 1 Name</t>
   </si>
@@ -542,6 +543,9 @@
   </si>
   <si>
     <t xml:space="preserve">SC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU, Other, POS</t>
   </si>
   <si>
     <t xml:space="preserve">Set Botella Abierta Sin Cooler</t>
@@ -996,29 +1000,28 @@
   </sheetPr>
   <dimension ref="A1:U65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D46" activeCellId="0" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.9336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.0816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7704081632653"/>
     <col collapsed="false" hidden="true" max="12" min="7" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="1.48469387755102"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="64.2551020408163"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="1.35204081632653"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="63.5816326530612"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,7 +3310,7 @@
         <v>Posters HE/Innovacion/BET</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="18" t="s">
@@ -3355,7 +3358,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>22</v>
@@ -3413,7 +3416,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>79</v>
@@ -3473,7 +3476,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>82</v>
@@ -3533,10 +3536,10 @@
     </row>
     <row r="49" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C49" s="0" t="str">
         <f aca="false">B49</f>
@@ -3593,10 +3596,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C50" s="0" t="str">
         <f aca="false">B50</f>
@@ -3631,19 +3634,19 @@
         <v>27</v>
       </c>
       <c r="P50" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Q50" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="R50" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="S50" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="T50" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="U50" s="8" t="s">
         <v>33</v>
@@ -3654,17 +3657,17 @@
         <v>91</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="20" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>25</v>
@@ -3695,10 +3698,10 @@
         <v>95</v>
       </c>
       <c r="R51" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="S51" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="T51" s="19" t="s">
         <v>144</v>
@@ -3738,111 +3741,111 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>171</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3869,7 +3872,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3895,28 +3898,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3942,13 +3945,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed missing underscore in template that was causing failures
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX_SAND/Data/inbevtradmx_template_2.xlsx
+++ b/Projects/INBEVTRADMX_SAND/Data/inbevtradmx_template_2.xlsx
@@ -28,6 +28,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">template!$A$1:$U$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">template!$A$1:$U$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -386,7 +387,7 @@
     <t xml:space="preserve">Product Availability KPI: If in scene type "Cigarros" there is at least 1 facing for Category "Cigarros", then pass.</t>
   </si>
   <si>
-    <t xml:space="preserve">product type, Category, store_type, template_name</t>
+    <t xml:space="preserve">product_type, Category, store_type, template_name</t>
   </si>
   <si>
     <t xml:space="preserve">Cooler Vacío</t>
@@ -1027,9 +1028,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>19080</xdr:colOff>
+      <xdr:colOff>18720</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:rowOff>7560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1039,7 +1040,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6210000" cy="6354000"/>
+          <a:ext cx="6123960" cy="6353640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1073,31 +1074,30 @@
   </sheetPr>
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="T12" activeCellId="0" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.6632653061224"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="62.9081632653061"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="62.0969387755102"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3833,8 +3833,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.4795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.8061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3960,6 +3963,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3984,7 +3990,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4031,7 +4038,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed capitalization issues in template that were causing errors
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX_SAND/Data/inbevtradmx_template_2.xlsx
+++ b/Projects/INBEVTRADMX_SAND/Data/inbevtradmx_template_2.xlsx
@@ -29,6 +29,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">template!$A$1:$U$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -108,7 +110,7 @@
     <t xml:space="preserve">manufacturer_name</t>
   </si>
   <si>
-    <t xml:space="preserve">Category</t>
+    <t xml:space="preserve">category</t>
   </si>
   <si>
     <t xml:space="preserve">Categoria Tradicional</t>
@@ -384,10 +386,10 @@
     <t xml:space="preserve">MODELORAMA</t>
   </si>
   <si>
-    <t xml:space="preserve">Product Availability KPI: If in scene type "Cigarros" there is at least 1 facing for Category "Cigarros", then pass.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_type, Category, store_type, template_name</t>
+    <t xml:space="preserve">Product Availability KPI: If in scene type "Cigarros" there is at least 1 facing for category "Cigarros", then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, category, store_type, template_name</t>
   </si>
   <si>
     <t xml:space="preserve">Cooler Vacío</t>
@@ -411,7 +413,7 @@
     <t xml:space="preserve">Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the cooler for selected manufacturers and category. 100% purity target.</t>
   </si>
   <si>
-    <t xml:space="preserve">product_type, manufacturer_name, Category, store_type, template_name</t>
+    <t xml:space="preserve">product_type, manufacturer_name, category, store_type, template_name</t>
   </si>
   <si>
     <t xml:space="preserve">SKU</t>
@@ -1030,7 +1032,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>18720</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>6840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1040,7 +1042,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6123960" cy="6353640"/>
+          <a:ext cx="7095600" cy="6352920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1074,30 +1076,35 @@
   </sheetPr>
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="T12" activeCellId="0" sqref="T12"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="S16" activeCellId="0" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="62.0969387755102"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="81.8061224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="97.0612244897959"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.6887755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3833,11 +3840,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.8061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.5918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3964,7 +3971,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3990,8 +3997,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4037,9 +4044,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>